<commit_message>
foreign key candidacy edited
</commit_message>
<xml_diff>
--- a/storage/csv_files/global_posts.xlsx
+++ b/storage/csv_files/global_posts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>sn</t>
   </si>
@@ -175,12 +175,6 @@
   </si>
   <si>
     <t>Regional Youth Deputy Coordinator Africa</t>
-  </si>
-  <si>
-    <t>Deputy Youth Coordinator</t>
-  </si>
-  <si>
-    <t>Deputy Woman Coordinator</t>
   </si>
   <si>
     <t>is_national_wide</t>
@@ -996,18 +990,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,7 +1023,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1057,7 +1053,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B51" si="0">"2021"&amp;IF($A3&lt;10,"_0","_")&amp;$A3</f>
+        <f t="shared" ref="B3:B49" si="0">"2021"&amp;IF($A3&lt;10,"_0","_")&amp;$A3</f>
         <v>2021_02</v>
       </c>
       <c r="C3" t="s">
@@ -1075,7 +1071,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A51" si="1">A3+1</f>
+        <f t="shared" ref="A4:A49" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="str">
@@ -1303,7 +1299,7 @@
         <v>2021_13</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -1312,7 +1308,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1325,7 +1321,7 @@
         <v>2021_14</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -1334,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1347,7 +1343,7 @@
         <v>2021_15</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -1369,7 +1365,7 @@
         <v>2021_16</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -1391,7 +1387,7 @@
         <v>2021_17</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -1413,7 +1409,7 @@
         <v>2021_18</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -1435,7 +1431,7 @@
         <v>2021_19</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -1457,7 +1453,7 @@
         <v>2021_20</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -1479,7 +1475,7 @@
         <v>2021_21</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -1501,7 +1497,7 @@
         <v>2021_22</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -1523,7 +1519,7 @@
         <v>2021_23</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1545,7 +1541,7 @@
         <v>2021_24</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -1567,7 +1563,7 @@
         <v>2021_25</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1581,7 +1577,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" ref="A27" si="2">A26+1</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" t="str">
@@ -1589,7 +1585,7 @@
         <v>2021_26</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -1603,15 +1599,15 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>A26+1</f>
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>2021_26</v>
+        <v>2021_27</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -1626,14 +1622,14 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>2021_27</v>
+        <v>2021_28</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1648,14 +1644,14 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>2021_28</v>
+        <v>2021_29</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
@@ -1670,14 +1666,14 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>2021_30</v>
+      </c>
+      <c r="C31" t="s">
         <v>29</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>2021_29</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -1692,20 +1688,20 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>2021_30</v>
+        <v>2021_31</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1714,14 +1710,14 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>2021_31</v>
+        <v>2021_32</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
@@ -1736,20 +1732,20 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v>2021_32</v>
+        <v>2021_33</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1758,14 +1754,14 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>2021_33</v>
+        <v>2021_34</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -1780,20 +1776,20 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>2021_34</v>
+        <v>2021_35</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1802,14 +1798,14 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>2021_35</v>
+        <v>2021_36</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1824,14 +1820,14 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
-        <v>2021_36</v>
+        <v>2021_37</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
@@ -1846,14 +1842,14 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v>2021_37</v>
+        <v>2021_38</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1868,14 +1864,14 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
-        <v>2021_38</v>
+        <v>2021_39</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
@@ -1890,14 +1886,14 @@
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
-        <v>2021_39</v>
+        <v>2021_40</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
@@ -1912,14 +1908,14 @@
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
-        <v>2021_40</v>
+        <v>2021_41</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
@@ -1934,14 +1930,14 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
-        <v>2021_41</v>
+        <v>2021_42</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -1956,14 +1952,14 @@
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
-        <v>2021_42</v>
+        <v>2021_43</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -1978,14 +1974,14 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
-        <v>2021_43</v>
+        <v>2021_44</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -2000,14 +1996,14 @@
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
-        <v>2021_44</v>
+        <v>2021_45</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
@@ -2022,14 +2018,14 @@
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
-        <v>2021_45</v>
+        <v>2021_46</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
@@ -2044,14 +2040,14 @@
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
-        <v>2021_46</v>
+        <v>2021_47</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -2066,14 +2062,14 @@
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
-        <v>2021_47</v>
+        <v>2021_48</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -2082,50 +2078,6 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>2021_48</v>
-      </c>
-      <c r="C50" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="B51" t="str">
-        <f t="shared" si="0"/>
-        <v>2021_49</v>
-      </c>
-      <c r="C51" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51">
         <v>0</v>
       </c>
     </row>

</xml_diff>